<commit_message>
Première validation pour push sur GitHub
</commit_message>
<xml_diff>
--- a/Proforma/2018 05/Analyse PROF1108BLAGNC export TXT.xlsx
+++ b/Proforma/2018 05/Analyse PROF1108BLAGNC export TXT.xlsx
@@ -4397,10 +4397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q58"/>
+  <dimension ref="A2:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4510,77 +4510,77 @@
         <v>220</v>
       </c>
       <c r="I7">
-        <f ca="1">MATCH(I$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ref="I7:Q7" ca="1" si="0">MATCH(I$6,INDIRECT($D7), 0)</f>
         <v>6</v>
       </c>
       <c r="J7">
-        <f ca="1">MATCH(J$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
       <c r="K7">
-        <f ca="1">MATCH(K$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>34</v>
       </c>
       <c r="L7">
-        <f ca="1">MATCH(L$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>52</v>
       </c>
       <c r="M7">
-        <f ca="1">MATCH(M$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>191</v>
       </c>
       <c r="N7">
-        <f ca="1">MATCH(N$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>206</v>
       </c>
       <c r="O7">
-        <f ca="1">MATCH(O$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>220</v>
       </c>
       <c r="P7">
-        <f ca="1">MATCH(P$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>122</v>
       </c>
       <c r="Q7">
-        <f ca="1">MATCH(Q$6,INDIRECT($D7), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I8" t="str">
-        <f ca="1">IF(I7=$F7,"",I7-$F7)</f>
+        <f t="shared" ref="I8:Q8" ca="1" si="1">IF(I7=$F7,"",I7-$F7)</f>
         <v/>
       </c>
       <c r="J8">
-        <f ca="1">IF(J7=$F7,"",J7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
       <c r="K8">
-        <f ca="1">IF(K7=$F7,"",K7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
       <c r="L8">
-        <f ca="1">IF(L7=$F7,"",L7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>46</v>
       </c>
       <c r="M8">
-        <f ca="1">IF(M7=$F7,"",M7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>185</v>
       </c>
       <c r="N8">
-        <f ca="1">IF(N7=$F7,"",N7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>200</v>
       </c>
       <c r="O8">
-        <f ca="1">IF(O7=$F7,"",O7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>214</v>
       </c>
       <c r="P8">
-        <f ca="1">IF(P7=$F7,"",P7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>116</v>
       </c>
       <c r="Q8">
-        <f ca="1">IF(Q7=$F7,"",Q7-$F7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>130</v>
       </c>
     </row>
@@ -4614,77 +4614,77 @@
         <v>246</v>
       </c>
       <c r="I9">
-        <f ca="1">MATCH(I$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ref="I9:Q9" ca="1" si="2">MATCH(I$6,INDIRECT($D9), 0)</f>
         <v>19</v>
       </c>
       <c r="J9">
-        <f ca="1">MATCH(J$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>35</v>
       </c>
       <c r="K9">
-        <f ca="1">MATCH(K$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>51</v>
       </c>
       <c r="L9">
-        <f ca="1">MATCH(L$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>68</v>
       </c>
       <c r="M9">
-        <f ca="1">MATCH(M$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>213</v>
       </c>
       <c r="N9">
-        <f ca="1">MATCH(N$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>230</v>
       </c>
       <c r="O9">
-        <f ca="1">MATCH(O$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>246</v>
       </c>
       <c r="P9">
-        <f ca="1">MATCH(P$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>138</v>
       </c>
       <c r="Q9">
-        <f ca="1">MATCH(Q$6,INDIRECT($D9), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I10" t="str">
-        <f ca="1">IF(I9=$F9,"",I9-$F9)</f>
+        <f t="shared" ref="I10:Q10" ca="1" si="3">IF(I9=$F9,"",I9-$F9)</f>
         <v/>
       </c>
       <c r="J10">
-        <f ca="1">IF(J9=$F9,"",J9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>16</v>
       </c>
       <c r="K10">
-        <f ca="1">IF(K9=$F9,"",K9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>32</v>
       </c>
       <c r="L10">
-        <f ca="1">IF(L9=$F9,"",L9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>49</v>
       </c>
       <c r="M10">
-        <f ca="1">IF(M9=$F9,"",M9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>194</v>
       </c>
       <c r="N10">
-        <f ca="1">IF(N9=$F9,"",N9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>211</v>
       </c>
       <c r="O10">
-        <f ca="1">IF(O9=$F9,"",O9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>227</v>
       </c>
       <c r="P10">
-        <f ca="1">IF(P9=$F9,"",P9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>119</v>
       </c>
       <c r="Q10">
-        <f ca="1">IF(Q9=$F9,"",Q9-$F9)</f>
+        <f t="shared" ca="1" si="3"/>
         <v>135</v>
       </c>
     </row>
@@ -4718,77 +4718,77 @@
         <v>192</v>
       </c>
       <c r="I11">
-        <f ca="1">MATCH(I$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ref="I11:Q11" ca="1" si="4">MATCH(I$6,INDIRECT($D11), 0)</f>
         <v>22</v>
       </c>
       <c r="J11">
-        <f ca="1">MATCH(J$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>29</v>
       </c>
       <c r="K11">
-        <f ca="1">MATCH(K$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>35</v>
       </c>
       <c r="L11">
-        <f ca="1">MATCH(L$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>44</v>
       </c>
       <c r="M11">
-        <f ca="1">MATCH(M$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>179</v>
       </c>
       <c r="N11">
-        <f ca="1">MATCH(N$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>186</v>
       </c>
       <c r="O11">
-        <f ca="1">MATCH(O$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>192</v>
       </c>
       <c r="P11">
-        <f ca="1">MATCH(P$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>142</v>
       </c>
       <c r="Q11">
-        <f ca="1">MATCH(Q$6,INDIRECT($D11), 0)</f>
+        <f t="shared" ca="1" si="4"/>
         <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I12" t="str">
-        <f ca="1">IF(I11=$F11,"",I11-$F11)</f>
+        <f t="shared" ref="I12:Q12" ca="1" si="5">IF(I11=$F11,"",I11-$F11)</f>
         <v/>
       </c>
       <c r="J12">
-        <f ca="1">IF(J11=$F11,"",J11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>7</v>
       </c>
       <c r="K12">
-        <f ca="1">IF(K11=$F11,"",K11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>13</v>
       </c>
       <c r="L12">
-        <f ca="1">IF(L11=$F11,"",L11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>22</v>
       </c>
       <c r="M12">
-        <f ca="1">IF(M11=$F11,"",M11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>157</v>
       </c>
       <c r="N12">
-        <f ca="1">IF(N11=$F11,"",N11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>164</v>
       </c>
       <c r="O12">
-        <f ca="1">IF(O11=$F11,"",O11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>170</v>
       </c>
       <c r="P12">
-        <f ca="1">IF(P11=$F11,"",P11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>120</v>
       </c>
       <c r="Q12">
-        <f ca="1">IF(Q11=$F11,"",Q11-$F11)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>127</v>
       </c>
     </row>
@@ -4821,35 +4821,35 @@
         <v>Ligne</v>
       </c>
       <c r="J19" s="3" t="str">
-        <f t="shared" ref="J19:Q19" si="0">J6</f>
+        <f t="shared" ref="J19:Q19" si="6">J6</f>
         <v>Modèle</v>
       </c>
       <c r="K19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Code pièce</v>
       </c>
       <c r="L19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Couleur</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Taille</v>
       </c>
       <c r="N19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Quantité</v>
       </c>
       <c r="O19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Prix unitaire</v>
       </c>
       <c r="P19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Montant</v>
       </c>
       <c r="Q19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Libellé</v>
       </c>
     </row>
@@ -4878,43 +4878,43 @@
         <v>1</v>
       </c>
       <c r="G20" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F20&amp;":A"&amp;(F20+5000)</f>
+        <f t="shared" ref="G20:G57" ca="1" si="7">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F20&amp;":A"&amp;(F20+5000)</f>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:Q35" ca="1" si="1">INDEX(INDIRECT($G20),OFFSET(INDIRECT($E20), 0, COLUMN(I20)-1)+$B20-1)</f>
+        <f t="shared" ref="I20:Q35" ca="1" si="8">INDEX(INDIRECT($G20),OFFSET(INDIRECT($E20), 0, COLUMN(I20)-1)+$B20-1)</f>
         <v>18</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS04 </v>
       </c>
       <c r="L20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>3</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6</v>
       </c>
       <c r="O20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.03</v>
       </c>
       <c r="P20">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>42.18</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN FAUX CUIR POMPON </v>
       </c>
     </row>
@@ -4928,7 +4928,7 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:C58" ca="1" si="2">OFFSET(INDEX($A:$A,$D21), 0, 2)</f>
+        <f ca="1">OFFSET(INDEX($A:$A,$D21), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D21">
@@ -4936,7 +4936,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E58" ca="1" si="3">"A" &amp; D21</f>
+        <f t="shared" ref="E21:E57" ca="1" si="9">"A" &amp; D21</f>
         <v>A7</v>
       </c>
       <c r="F21">
@@ -4944,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F21&amp;":A"&amp;(F21+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I21">
@@ -4952,49 +4952,49 @@
         <v>19</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS04 </v>
       </c>
       <c r="L21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>26</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
       <c r="O21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.03</v>
       </c>
       <c r="P21">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>56.24</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN FAUX CUIR POMPON </v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" ref="A22:A34" ca="1" si="4">IF(B21=C21,A21+1,A21)</f>
+        <f t="shared" ref="A22:A34" ca="1" si="10">IF(B21=C21,A21+1,A21)</f>
         <v>1</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B33" ca="1" si="5">IF(A22=A21,B21+1,1)</f>
+        <f t="shared" ref="B22:B33" ca="1" si="11">IF(A22=A21,B21+1,1)</f>
         <v>3</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D22), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D22">
@@ -5002,7 +5002,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F22">
@@ -5010,57 +5010,57 @@
         <v>1</v>
       </c>
       <c r="G22" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F22&amp;":A"&amp;(F22+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:Q37" ca="1" si="6">INDEX(INDIRECT($G22),OFFSET(INDIRECT($E22), 0, COLUMN(I22)-1)+$B22-1)</f>
+        <f t="shared" ref="I22:Q37" ca="1" si="12">INDEX(INDIRECT($G22),OFFSET(INDIRECT($E22), 0, COLUMN(I22)-1)+$B22-1)</f>
         <v>20</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">PES00 </v>
       </c>
       <c r="L22">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>54</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N22">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
       <c r="O22">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>16.2</v>
       </c>
       <c r="P22">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>162</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN CUIR </v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>4</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D23), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D23">
@@ -5068,7 +5068,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F23">
@@ -5076,57 +5076,57 @@
         <v>1</v>
       </c>
       <c r="G23" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F23&amp;":A"&amp;(F23+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I23">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>22</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>14</v>
       </c>
       <c r="O23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.39</v>
       </c>
       <c r="P23">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>103.46</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN CORDE </v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D24), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D24">
@@ -5134,7 +5134,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F24">
@@ -5142,57 +5142,57 @@
         <v>1</v>
       </c>
       <c r="G24" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F24&amp;":A"&amp;(F24+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I24">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>23</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>9</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
       <c r="O24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.39</v>
       </c>
       <c r="P24">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>73.900000000000006</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN CORDE </v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>6</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D25), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D25">
@@ -5200,7 +5200,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F25">
@@ -5208,57 +5208,57 @@
         <v>1</v>
       </c>
       <c r="G25" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F25&amp;":A"&amp;(F25+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I25">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>21</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>54</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>30</v>
       </c>
       <c r="O25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.39</v>
       </c>
       <c r="P25">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>221.7</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN CORDE </v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>7</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D26), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D26">
@@ -5266,7 +5266,7 @@
         <v>7</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F26">
@@ -5274,57 +5274,57 @@
         <v>1</v>
       </c>
       <c r="G26" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F26&amp;":A"&amp;(F26+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I26">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>24</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESG000 </v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>76</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
       <c r="O26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.39</v>
       </c>
       <c r="P26">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>73.900000000000006</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES LONGUES EN CORDE </v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>8</v>
       </c>
       <c r="C27">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D27), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D27">
@@ -5332,7 +5332,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F27">
@@ -5340,57 +5340,57 @@
         <v>1</v>
       </c>
       <c r="G27" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F27&amp;":A"&amp;(F27+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I27">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>25</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS01 </v>
       </c>
       <c r="L27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
       <c r="O27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>7.75</v>
       </c>
       <c r="P27">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>77.5</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN FAUX CUIR MARTELÉ </v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>9</v>
       </c>
       <c r="C28">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D28), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D28">
@@ -5398,7 +5398,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F28">
@@ -5406,57 +5406,57 @@
         <v>1</v>
       </c>
       <c r="G28" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F28&amp;":A"&amp;(F28+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I28">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>26</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS04 </v>
       </c>
       <c r="L28">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>26</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N28">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
       <c r="O28">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.05</v>
       </c>
       <c r="P28">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>48.4</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN FAUX CUIR POMPON </v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>10</v>
       </c>
       <c r="C29">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D29), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D29">
@@ -5464,7 +5464,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F29">
@@ -5472,57 +5472,57 @@
         <v>1</v>
       </c>
       <c r="G29" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F29&amp;":A"&amp;(F29+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I29">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>27</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS54 </v>
       </c>
       <c r="L29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>75</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>4</v>
       </c>
       <c r="O29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>16.32</v>
       </c>
       <c r="P29">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>65.28</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN FAUX CUIR CLOUS ÉMAILLÉS </v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>11</v>
       </c>
       <c r="C30">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D30), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D30">
@@ -5530,7 +5530,7 @@
         <v>7</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F30">
@@ -5538,57 +5538,57 @@
         <v>1</v>
       </c>
       <c r="G30" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F30&amp;":A"&amp;(F30+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I30">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>28</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ECS54 </v>
       </c>
       <c r="L30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>479</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>4</v>
       </c>
       <c r="O30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>16.32</v>
       </c>
       <c r="P30">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>65.28</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN FAUX CUIR CLOUS ÉMAILLÉS </v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>12</v>
       </c>
       <c r="C31">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D31), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D31">
@@ -5596,7 +5596,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F31">
@@ -5604,57 +5604,57 @@
         <v>1</v>
       </c>
       <c r="G31" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F31&amp;":A"&amp;(F31+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I31">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>29</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L31">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>8</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N31">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>12</v>
       </c>
       <c r="O31">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.28</v>
       </c>
       <c r="P31">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>75.36</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>13</v>
       </c>
       <c r="C32">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D32), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D32">
@@ -5662,7 +5662,7 @@
         <v>7</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F32">
@@ -5670,57 +5670,57 @@
         <v>1</v>
       </c>
       <c r="G32" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F32&amp;":A"&amp;(F32+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I32">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>30</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>9</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>12</v>
       </c>
       <c r="O32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.28</v>
       </c>
       <c r="P32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>75.36</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>1</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="11"/>
         <v>14</v>
       </c>
       <c r="C33">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D33), 0, 2)</f>
         <v>14</v>
       </c>
       <c r="D33">
@@ -5728,7 +5728,7 @@
         <v>7</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A7</v>
       </c>
       <c r="F33">
@@ -5736,49 +5736,49 @@
         <v>1</v>
       </c>
       <c r="G33" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F33&amp;":A"&amp;(F33+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I33">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>31</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>39</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>10</v>
       </c>
       <c r="O33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.28</v>
       </c>
       <c r="P33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>62.8</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="10"/>
         <v>2</v>
       </c>
       <c r="B34">
@@ -5786,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D34), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D34">
@@ -5794,7 +5794,7 @@
         <v>9</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F34">
@@ -5802,57 +5802,57 @@
         <v>221</v>
       </c>
       <c r="G34" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F34&amp;":A"&amp;(F34+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I34">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>32</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>54</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>20</v>
       </c>
       <c r="O34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.28</v>
       </c>
       <c r="P34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>125.6</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" ref="A35:A55" ca="1" si="7">IF(B34=C34,A34+1,A34)</f>
+        <f t="shared" ref="A35:A55" ca="1" si="13">IF(B34=C34,A34+1,A34)</f>
         <v>2</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:B41" ca="1" si="8">IF(A35=A34,B34+1,1)</f>
+        <f t="shared" ref="B35:B41" ca="1" si="14">IF(A35=A34,B34+1,1)</f>
         <v>2</v>
       </c>
       <c r="C35">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D35), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D35">
@@ -5860,7 +5860,7 @@
         <v>9</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F35">
@@ -5868,57 +5868,57 @@
         <v>221</v>
       </c>
       <c r="G35" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F35&amp;":A"&amp;(F35+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I35">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>33</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>55</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>20</v>
       </c>
       <c r="O35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>6.28</v>
       </c>
       <c r="P35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v>125.6</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>3</v>
       </c>
       <c r="C36">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D36), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D36">
@@ -5926,7 +5926,7 @@
         <v>9</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F36">
@@ -5934,57 +5934,57 @@
         <v>221</v>
       </c>
       <c r="G36" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F36&amp;":A"&amp;(F36+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I36">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>34</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">HLESGC00 </v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">ROS00 </v>
       </c>
       <c r="L36">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>76</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N36">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>10</v>
       </c>
       <c r="O36">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>6.28</v>
       </c>
       <c r="P36">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>62.8</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">ANSES COURTES EN CORDE </v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>4</v>
       </c>
       <c r="C37">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D37), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D37">
@@ -5992,7 +5992,7 @@
         <v>9</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F37">
@@ -6000,57 +6000,57 @@
         <v>221</v>
       </c>
       <c r="G37" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F37&amp;":A"&amp;(F37+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I37">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>35</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">OBAGB002 </v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">EVS00 </v>
       </c>
       <c r="L37">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>17</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">UNICA </v>
       </c>
       <c r="N37">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>6</v>
       </c>
       <c r="O37">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>14.4</v>
       </c>
       <c r="P37">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v>86.4</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="12"/>
         <v xml:space="preserve">CORPS O BAG MINI EVA COMPOUND </v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>5</v>
       </c>
       <c r="C38">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D38), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D38">
@@ -6058,7 +6058,7 @@
         <v>9</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F38">
@@ -6066,57 +6066,57 @@
         <v>221</v>
       </c>
       <c r="G38" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F38&amp;":A"&amp;(F38+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I38">
-        <f t="shared" ref="I38:Q53" ca="1" si="9">INDEX(INDIRECT($G38),OFFSET(INDIRECT($E38), 0, COLUMN(I38)-1)+$B38-1)</f>
+        <f t="shared" ref="I38:Q53" ca="1" si="15">INDEX(INDIRECT($G38),OFFSET(INDIRECT($E38), 0, COLUMN(I38)-1)+$B38-1)</f>
         <v>2</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OBAGK700 </v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">TESI8 </v>
       </c>
       <c r="L38">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">M </v>
       </c>
       <c r="N38">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>6</v>
       </c>
       <c r="O38">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>0.54</v>
       </c>
       <c r="P38">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.24</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">PACKAGING SACHETS EN TISSU TNT </v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>6</v>
       </c>
       <c r="C39">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D39), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D39">
@@ -6124,7 +6124,7 @@
         <v>9</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F39">
@@ -6132,57 +6132,57 @@
         <v>221</v>
       </c>
       <c r="G39" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F39&amp;":A"&amp;(F39+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I39">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>1</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L39">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
       <c r="M39" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N39">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="O39">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P39">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>28.8</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B40">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>7</v>
       </c>
       <c r="C40">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D40), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D40">
@@ -6190,7 +6190,7 @@
         <v>9</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F40">
@@ -6198,57 +6198,57 @@
         <v>221</v>
       </c>
       <c r="G40" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F40&amp;":A"&amp;(F40+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I40">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>36</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L40">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N40">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="O40">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P40">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>28.8</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="14"/>
         <v>8</v>
       </c>
       <c r="C41">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D41), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D41">
@@ -6256,7 +6256,7 @@
         <v>9</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F41">
@@ -6264,49 +6264,49 @@
         <v>221</v>
       </c>
       <c r="G41" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F41&amp;":A"&amp;(F41+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I41">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L41">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N41">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>20</v>
       </c>
       <c r="O41">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P41">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>72</v>
       </c>
       <c r="Q41" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B42">
@@ -6314,7 +6314,7 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D42), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D42">
@@ -6322,7 +6322,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F42">
@@ -6330,57 +6330,57 @@
         <v>221</v>
       </c>
       <c r="G42" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F42&amp;":A"&amp;(F42+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I42">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>4</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L42">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>12</v>
       </c>
       <c r="M42" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N42">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="O42">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P42">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>28.8</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:B45" ca="1" si="10">IF(A43=A42,B42+1,1)</f>
+        <f t="shared" ref="B43:B45" ca="1" si="16">IF(A43=A42,B42+1,1)</f>
         <v>10</v>
       </c>
       <c r="C43">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D43), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D43">
@@ -6388,7 +6388,7 @@
         <v>9</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F43">
@@ -6396,57 +6396,57 @@
         <v>221</v>
       </c>
       <c r="G43" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F43&amp;":A"&amp;(F43+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I43">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>5</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L43">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>13</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N43">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="O43">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P43">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>36</v>
       </c>
       <c r="Q43" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="16"/>
         <v>11</v>
       </c>
       <c r="C44">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D44), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D44">
@@ -6454,7 +6454,7 @@
         <v>9</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F44">
@@ -6462,57 +6462,57 @@
         <v>221</v>
       </c>
       <c r="G44" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F44&amp;":A"&amp;(F44+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I44">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>6</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L44">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N44">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="O44">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P44">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>28.8</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="16"/>
         <v>12</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D45), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D45">
@@ -6520,7 +6520,7 @@
         <v>9</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F45">
@@ -6528,49 +6528,49 @@
         <v>221</v>
       </c>
       <c r="G45" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F45&amp;":A"&amp;(F45+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I45">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>7</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L45">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>22</v>
       </c>
       <c r="M45" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N45">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="O45">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P45">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>28.8</v>
       </c>
       <c r="Q45" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B46">
@@ -6578,7 +6578,7 @@
         <v>13</v>
       </c>
       <c r="C46">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D46), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D46">
@@ -6586,7 +6586,7 @@
         <v>9</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F46">
@@ -6594,57 +6594,57 @@
         <v>221</v>
       </c>
       <c r="G46" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F46&amp;":A"&amp;(F46+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I46">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L46">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>41</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N46">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>12</v>
       </c>
       <c r="O46">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P46">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>43.2</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B47">
-        <f t="shared" ref="B47" ca="1" si="11">IF(A47=A46,B46+1,1)</f>
+        <f t="shared" ref="B47" ca="1" si="17">IF(A47=A46,B46+1,1)</f>
         <v>14</v>
       </c>
       <c r="C47">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D47), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D47">
@@ -6652,7 +6652,7 @@
         <v>9</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F47">
@@ -6660,57 +6660,57 @@
         <v>221</v>
       </c>
       <c r="G47" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F47&amp;":A"&amp;(F47+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I47">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L47">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>53</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N47">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="O47">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P47">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>36</v>
       </c>
       <c r="Q47" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:B50" ca="1" si="12">IF(A48=A47,B47+1,1)</f>
+        <f t="shared" ref="B48:B50" ca="1" si="18">IF(A48=A47,B47+1,1)</f>
         <v>15</v>
       </c>
       <c r="C48">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D48), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D48">
@@ -6718,7 +6718,7 @@
         <v>9</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F48">
@@ -6726,57 +6726,57 @@
         <v>221</v>
       </c>
       <c r="G48" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F48&amp;":A"&amp;(F48+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I48">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L48">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>55</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N48">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>20</v>
       </c>
       <c r="O48">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P48">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>72</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>2</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="18"/>
         <v>16</v>
       </c>
       <c r="C49">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D49), 0, 2)</f>
         <v>16</v>
       </c>
       <c r="D49">
@@ -6784,7 +6784,7 @@
         <v>9</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A9</v>
       </c>
       <c r="F49">
@@ -6792,57 +6792,57 @@
         <v>221</v>
       </c>
       <c r="G49" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F49&amp;":A"&amp;(F49+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A221:A5221</v>
       </c>
       <c r="I49">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>11</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L49">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>59</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N49">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>20</v>
       </c>
       <c r="O49">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P49">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>72</v>
       </c>
       <c r="Q49" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" ref="A50" ca="1" si="13">IF(B49=C49,A49+1,A49)</f>
+        <f t="shared" ref="A50" ca="1" si="19">IF(B49=C49,A49+1,A49)</f>
         <v>3</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="18"/>
         <v>1</v>
       </c>
       <c r="C50">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D50), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D50">
@@ -6850,7 +6850,7 @@
         <v>11</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F50">
@@ -6858,57 +6858,57 @@
         <v>467</v>
       </c>
       <c r="G50" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F50&amp;":A"&amp;(F50+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I50">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>12</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L50">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>71</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N50">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>20</v>
       </c>
       <c r="O50">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P50">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>72</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>3</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51:B55" ca="1" si="14">IF(A51=A50,B50+1,1)</f>
+        <f t="shared" ref="B51:B55" ca="1" si="20">IF(A51=A50,B50+1,1)</f>
         <v>2</v>
       </c>
       <c r="C51">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D51), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D51">
@@ -6916,7 +6916,7 @@
         <v>11</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F51">
@@ -6924,57 +6924,57 @@
         <v>467</v>
       </c>
       <c r="G51" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F51&amp;":A"&amp;(F51+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I51">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>13</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K51" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L51">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>76</v>
       </c>
       <c r="M51" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N51">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>12</v>
       </c>
       <c r="O51">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P51">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>43.2</v>
       </c>
       <c r="Q51" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>3</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="20"/>
         <v>3</v>
       </c>
       <c r="C52">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D52), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D52">
@@ -6982,7 +6982,7 @@
         <v>11</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F52">
@@ -6990,57 +6990,57 @@
         <v>467</v>
       </c>
       <c r="G52" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F52&amp;":A"&amp;(F52+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I52">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K52" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L52">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>86</v>
       </c>
       <c r="M52" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N52">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>16</v>
       </c>
       <c r="O52">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P52">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>57.6</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>3</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="20"/>
         <v>4</v>
       </c>
       <c r="C53">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D53), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D53">
@@ -7048,7 +7048,7 @@
         <v>11</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F53">
@@ -7056,57 +7056,57 @@
         <v>467</v>
       </c>
       <c r="G53" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F53&amp;":A"&amp;(F53+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I53">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>15</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K53" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L53">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>88</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N53">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="O53">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3.6</v>
       </c>
       <c r="P53">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v>36</v>
       </c>
       <c r="Q53" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="15"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>3</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="20"/>
         <v>5</v>
       </c>
       <c r="C54">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D54), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D54">
@@ -7114,7 +7114,7 @@
         <v>11</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F54">
@@ -7122,57 +7122,57 @@
         <v>467</v>
       </c>
       <c r="G54" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F54&amp;":A"&amp;(F54+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I54">
-        <f t="shared" ref="I54:Q58" ca="1" si="15">INDEX(INDIRECT($G54),OFFSET(INDIRECT($E54), 0, COLUMN(I54)-1)+$B54-1)</f>
+        <f t="shared" ref="I54:Q57" ca="1" si="21">INDEX(INDIRECT($G54),OFFSET(INDIRECT($E54), 0, COLUMN(I54)-1)+$B54-1)</f>
         <v>16</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L54">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>96</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N54">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>14</v>
       </c>
       <c r="O54">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>3.6</v>
       </c>
       <c r="P54">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>50.4</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>3</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="20"/>
         <v>6</v>
       </c>
       <c r="C55">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D55), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D55">
@@ -7180,7 +7180,7 @@
         <v>11</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F55">
@@ -7188,65 +7188,65 @@
         <v>467</v>
       </c>
       <c r="G55" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F55&amp;":A"&amp;(F55+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I55">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>17</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">OCLKS007 </v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="L55">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>484</v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">S </v>
       </c>
       <c r="N55">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>10</v>
       </c>
       <c r="O55">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>3.6</v>
       </c>
       <c r="P55">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>36</v>
       </c>
       <c r="Q55" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">O CLOCK BRACELET COVER EN SILICONE </v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" ref="A56:A58" ca="1" si="16">IF(B55=C55,A55+1,A55)</f>
+        <f t="shared" ref="A56:A57" ca="1" si="22">IF(B55=C55,A55+1,A55)</f>
         <v>3</v>
       </c>
       <c r="B56">
-        <f t="shared" ref="B56:B58" ca="1" si="17">IF(A56=A55,B55+1,1)</f>
+        <f t="shared" ref="B56:B57" ca="1" si="23">IF(A56=A55,B55+1,1)</f>
         <v>7</v>
       </c>
       <c r="C56">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D56), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56:D58" ca="1" si="18">MATCH(A56,A:A,0)</f>
+        <f ca="1">MATCH(A56,A:A,0)</f>
         <v>11</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A11</v>
       </c>
       <c r="F56">
@@ -7254,65 +7254,65 @@
         <v>467</v>
       </c>
       <c r="G56" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F56&amp;":A"&amp;(F56+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A467:A5467</v>
       </c>
       <c r="I56">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>37</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">000_SPTRASP </v>
       </c>
       <c r="L56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">002488 O BAG STORE BLAGNAC </v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">Taille </v>
       </c>
       <c r="N56">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>3.6</v>
       </c>
       <c r="O56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SOFEA </v>
       </c>
       <c r="P56">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>32</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">DÉBIT FRAIS DE TRANSPORT </v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="22"/>
         <v>4</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="23"/>
         <v>1</v>
       </c>
       <c r="C57">
-        <f t="shared" ca="1" si="2"/>
+        <f ca="1">OFFSET(INDEX($A:$A,$D57), 0, 2)</f>
         <v>7</v>
       </c>
       <c r="D57">
-        <f t="shared" ca="1" si="18"/>
+        <f ca="1">MATCH(A57,A:A,0)</f>
         <v>57</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="9"/>
         <v>A57</v>
       </c>
       <c r="F57">
@@ -7320,110 +7320,44 @@
         <v>1</v>
       </c>
       <c r="G57" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F57&amp;":A"&amp;(F57+5000)</f>
+        <f t="shared" ca="1" si="7"/>
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="I57">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>37</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SIS01 </v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">000_SPTRASP </v>
       </c>
       <c r="L57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">002488 O BAG STORE BLAGNAC </v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">Taille </v>
       </c>
       <c r="N57">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v>3.6</v>
       </c>
       <c r="O57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">SOFEA </v>
       </c>
       <c r="P57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">32,00 32,000 1,000 </v>
       </c>
       <c r="Q57" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="21"/>
         <v xml:space="preserve">DÉBIT FRAIS DE TRANSPORT </v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <f t="shared" ca="1" si="16"/>
-        <v>4</v>
-      </c>
-      <c r="B58">
-        <f t="shared" ca="1" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="C58" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="D58">
-        <f t="shared" ca="1" si="18"/>
-        <v>58</v>
-      </c>
-      <c r="E58" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>A58</v>
-      </c>
-      <c r="F58">
-        <f ca="1">OFFSET(INDEX($A:$A,$D58), 0, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="G58" t="str">
-        <f ca="1">"'"&amp;nomOngletDonnées&amp;"'!A"&amp;F58&amp;":A"&amp;(F58+5000)</f>
-        <v>'Données'!A1:A5001</v>
-      </c>
-      <c r="I58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="J58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="K58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="L58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="M58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="N58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="O58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="P58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
-      </c>
-      <c r="Q58">
-        <f t="shared" ca="1" si="15"/>
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>